<commit_message>
Adding the table of requirements Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS/CYRS_Cross_review.xlsx
+++ b/Input documents/CYRS/CYRS_Cross_review.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Name of file</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Reflecting the Added requirements into the constraint table</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>May Alaa</t>
   </si>
 </sst>
 </file>
@@ -154,43 +160,7 @@
     <cellStyle name="Excel Built-in Accent3" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -466,64 +436,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>